<commit_message>
Added  description tab to the Excel reporting templates
</commit_message>
<xml_diff>
--- a/excel_reporting_templates/BusinessPartnerCertificate-1.0.0-schema-reporting_template.xlsx
+++ b/excel_reporting_templates/BusinessPartnerCertificate-1.0.0-schema-reporting_template.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="semantic_aspect_model_schema" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="possible_values" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="description" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="metadata" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,11 +57,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,177 +436,101 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="50" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
-    <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="50" customWidth="1" min="6" max="6"/>
-    <col width="50" customWidth="1" min="7" max="7"/>
-    <col width="50" customWidth="1" min="8" max="8"/>
-    <col width="50" customWidth="1" min="9" max="9"/>
-    <col width="50" customWidth="1" min="10" max="10"/>
-    <col width="50" customWidth="1" min="11" max="11"/>
-    <col width="50" customWidth="1" min="12" max="12"/>
-    <col width="50" customWidth="1" min="13" max="13"/>
-    <col width="50" customWidth="1" min="14" max="14"/>
-    <col width="50" customWidth="1" min="15" max="15"/>
+    <col width="25.2" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="27.6" customWidth="1" min="3" max="3"/>
+    <col width="21.6" customWidth="1" min="4" max="4"/>
+    <col width="20.4" customWidth="1" min="5" max="5"/>
+    <col width="38.4" customWidth="1" min="6" max="6"/>
+    <col width="40.8" customWidth="1" min="7" max="7"/>
+    <col width="10.8" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="7.199999999999999" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="27.6" customWidth="1" min="12" max="12"/>
+    <col width="26.4" customWidth="1" min="13" max="13"/>
+    <col width="9.6" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>The provided regular expression ensures that the BPNL is composed of prefix 'BPNL', 10 digits and two alphanumeric letters.</t>
+          <t>businessPartnerNumber</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
+          <t>type_certificateType</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>type_certificateVersion</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
+          <t>registrationNumber</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>areaOfApplication</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>The provided regular expression ensures that the BPNS is composed of prefix 'BPNS', 10 digits and two alphanumeric letters.</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
+          <t>enclosedSites[0]_enclosedSiteBpn</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>enclosedSites[0]_areaOfApplication</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Describes a property which contains the date in english format.</t>
+          <t>validFrom</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Describes a property which contains the date in english format.</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>The provided regular expression ensures that the BPNL is composed of prefix 'BPNL', 10 digits and two alphanumeric letters.</t>
+          <t>validUntil</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>issuer</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>The possible trust level values of certificate</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
+          <t>trustLevel</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>validator_validatorName</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>The provided regular expression ensures that the BPNL is composed of prefix 'BPNL', 10 digits and two alphanumeric letters.</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>The provided regular expression ensures that the BPNL is composed of prefix 'BPNL', 10 digits and two alphanumeric letters.</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Describes a Property which contains plain text. This is intended exclusively for human readable strings, not for identifiers, measurement values, etc.</t>
+          <t>validator_validatorBpn</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>uploader</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>documentID</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>businessPartnerNumber</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>type_certificateType</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>type_certificateVersion</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>registrationNumber</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>areaOfApplication</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>enclosedSites_enclosedSiteBpn</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>enclosedSites_areaOfApplication</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>validFrom</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>validUntil</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>issuer</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>trustLevel</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>validator_validatorName</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>validator_validatorBpn</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>uploader</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>documentID</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
     <row r="3"/>
     <row r="4"/>
     <row r="5"/>
@@ -1603,7 +1529,10 @@
     <row r="998"/>
     <row r="999"/>
   </sheetData>
-  <dataValidations count="997">
+  <dataValidations count="998">
+    <dataValidation sqref="K2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>=possible_values!$A$2:$A$5</formula1>
+    </dataValidation>
     <dataValidation sqref="K3" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>=possible_values!$A$2:$A$5</formula1>
     </dataValidation>
@@ -4652,4 +4581,309 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="36" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="36" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Possible Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>businessPartnerNumber</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The BPN of the certified legal entity </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>type_certificateType</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Type of the certificate as defined on the document,valid types are registered at BPN metadatacontroller</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>type_certificateVersion</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Version of the certificate as defined on the document, usually the specific version of a certification standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>registrationNumber</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Registration number of the certificate as defined on the certificate</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>areaOfApplication</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Details on which areas / application types a certificate is valid for a company</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>enclosedSites[0]_enclosedSiteBpn</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The BPN of an enclosed site </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>enclosedSites[0]_areaOfApplication</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Details on which areas / application types a certificate is valid for a company</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>validFrom</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Valid from date as defined on the certificate.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>validUntil</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Valid valid until as defined on the certificate. If certificate never expires value until expected to be 9999-12-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>issuer</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The BPN of the issuing authority e.g. TUEV Sued </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>trustLevel</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>The trust level of the given certificate - none,low, high, trusted</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['none', 'low', 'high', 'trusted']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>validator_validatorName</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>The optional name of the data service provider who validated the given certificate</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>validator_validatorBpn</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>The BPN of the data service provider who validated the given certificate</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>uploader</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>The BPN of the business partner who originally provided the certifcate data or document e.g. Mercedes Benz AG</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>documentID</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>The id of the certificate document as stored by the data service provider for physical download via API</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>basedOnCommit</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>aec6f34c9336d73dbc54e5762a672b79c59fae14</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>commitHtmlUrl</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://github.com/dataspacesolutions/sldt-semantic-models/commit/aec6f34c9336d73dbc54e5762a672b79c59fae14</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>commitDate</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-03-28 08:02:07+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>commitMessage</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>add BusinessPartnerCertificate v3.1.0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>